<commit_message>
cambio nombre  insprector a reporte
</commit_message>
<xml_diff>
--- a/reports/tpFijo.xlsx
+++ b/reports/tpFijo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="INF.0000" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="143">
   <si>
     <t xml:space="preserve">NIT. 901.356.384 – 1</t>
   </si>
@@ -524,6 +524,12 @@
   </si>
   <si>
     <t xml:space="preserve">OTRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cargo:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inspector</t>
   </si>
   <si>
     <t xml:space="preserve">CC</t>
@@ -1485,10 +1491,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>45360</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>685080</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1502,7 +1508,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6674760" cy="1682280"/>
+          <a:ext cx="6673680" cy="1681920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1528,9 +1534,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>640440</xdr:colOff>
+      <xdr:colOff>640080</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:rowOff>88920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1544,7 +1550,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="4678920" cy="1327680"/>
+          <a:ext cx="4681080" cy="1327320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1566,24 +1572,24 @@
   </sheetPr>
   <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I48" activeCellId="0" sqref="I48"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J73" activeCellId="0" sqref="J73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="9" style="1" width="17.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="14.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="26" min="17" style="1" width="11.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="9.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="2.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="3.28"/>
@@ -3241,7 +3247,9 @@
         <v>125</v>
       </c>
       <c r="D77" s="89"/>
-      <c r="E77" s="90"/>
+      <c r="E77" s="92" t="s">
+        <v>130</v>
+      </c>
       <c r="F77" s="90"/>
       <c r="G77" s="90"/>
       <c r="H77" s="90"/>
@@ -3263,13 +3271,17 @@
       <c r="B78" s="94"/>
       <c r="C78" s="94"/>
       <c r="D78" s="94"/>
-      <c r="E78" s="90"/>
-      <c r="F78" s="90"/>
-      <c r="G78" s="90"/>
-      <c r="H78" s="90"/>
-      <c r="I78" s="90"/>
+      <c r="E78" s="92" t="s">
+        <v>132</v>
+      </c>
+      <c r="F78" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="G78" s="15"/>
+      <c r="H78" s="15"/>
+      <c r="I78" s="15"/>
       <c r="J78" s="95" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K78" s="93"/>
       <c r="L78" s="93"/>
@@ -3280,7 +3292,7 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="96" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B79" s="96"/>
       <c r="C79" s="96"/>
@@ -3317,7 +3329,7 @@
       <c r="P80" s="96"/>
     </row>
   </sheetData>
-  <mergeCells count="171">
+  <mergeCells count="173">
     <mergeCell ref="A1:G6"/>
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="N1:P1"/>
@@ -3484,10 +3496,12 @@
     <mergeCell ref="A72:D72"/>
     <mergeCell ref="E72:I72"/>
     <mergeCell ref="J72:P72"/>
-    <mergeCell ref="E73:I78"/>
+    <mergeCell ref="E73:I76"/>
     <mergeCell ref="J73:P76"/>
+    <mergeCell ref="F77:I77"/>
     <mergeCell ref="K77:P78"/>
     <mergeCell ref="A78:D78"/>
+    <mergeCell ref="F78:I78"/>
     <mergeCell ref="A79:P80"/>
   </mergeCells>
   <hyperlinks>
@@ -3511,11 +3525,11 @@
   </sheetPr>
   <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="3.57"/>
@@ -3651,7 +3665,7 @@
     </row>
     <row r="7" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="100" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B7" s="100"/>
       <c r="C7" s="100"/>
@@ -3691,7 +3705,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="101" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B9" s="101"/>
       <c r="C9" s="101"/>
@@ -3701,7 +3715,7 @@
       <c r="G9" s="101"/>
       <c r="H9" s="101"/>
       <c r="I9" s="101" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J9" s="101"/>
       <c r="K9" s="101"/>
@@ -3983,7 +3997,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="101" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B25" s="101"/>
       <c r="C25" s="101"/>
@@ -3993,7 +4007,7 @@
       <c r="G25" s="101"/>
       <c r="H25" s="101"/>
       <c r="I25" s="101" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="J25" s="101"/>
       <c r="K25" s="101"/>
@@ -4275,7 +4289,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="101" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B41" s="101"/>
       <c r="C41" s="101"/>
@@ -4583,7 +4597,7 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="101" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B58" s="101"/>
       <c r="C58" s="101"/>

</xml_diff>